<commit_message>
all tokens visible w/out connection. contract floorprice scaled to maxSupply
</commit_message>
<xml_diff>
--- a/bonding curve logic.xlsx
+++ b/bonding curve logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Praca\web3\turbo-launchpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7F9C6B-01D3-45CB-B684-A0DFC54F9D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECD1B1-185E-427B-A718-4E3A3C8D49D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B37AC876-497F-4A49-9875-044F50F94948}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Raise target</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>S (graduateThreshold)</t>
+  </si>
+  <si>
+    <t>floorprice=1000000000</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -243,7 +246,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -582,7 +585,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,14 +626,14 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2">
         <f>C2*1000000000000000000</f>
-        <v>1.2E+19</v>
+        <v>2.5E+19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -659,18 +662,19 @@
         <v>21</v>
       </c>
       <c r="C4" s="2">
-        <v>5.0000000000000001E-3</v>
+        <f>0.005*1000000000/C5</f>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="1">
         <f>1000000000000000000*C4/C$3</f>
-        <v>1923076923076.9231</v>
+        <v>384615384615384.63</v>
       </c>
       <c r="H4">
         <f>C4/C3</f>
-        <v>1.923076923076923E-6</v>
+        <v>3.8461538461538462E-4</v>
       </c>
       <c r="I4" s="6">
         <v>1.9999999999999999E-6</v>
@@ -684,14 +688,14 @@
         <v>14</v>
       </c>
       <c r="C5">
-        <v>1000000000</v>
+        <v>5000000</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1">
         <f>C5*1000000000000000000</f>
-        <v>1E+27</v>
+        <v>5.0000000000000005E+24</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -709,27 +713,27 @@
       </c>
       <c r="E6" s="1">
         <f>E5*C6</f>
-        <v>3.9999999999999999E+24</v>
+        <v>2.0000000000000004E+22</v>
       </c>
       <c r="F6">
         <f>C5*C6</f>
-        <v>4000000</v>
+        <v>20000</v>
       </c>
       <c r="H6">
         <f>2*C2/F6</f>
-        <v>6.0000000000000002E-6</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="I6">
         <f>C8/C3</f>
-        <v>4.6153846153846153E-6</v>
+        <v>1.9230769230769232E-3</v>
       </c>
       <c r="J6">
         <f>H6-I6</f>
-        <v>1.3846153846153848E-6</v>
+        <v>5.7692307692307687E-4</v>
       </c>
       <c r="K6">
         <f>J6*1000000000000000000</f>
-        <v>1384615384615.3848</v>
+        <v>576923076923076.88</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -759,22 +763,22 @@
       </c>
       <c r="C8">
         <f>C2*C4/C7</f>
-        <v>1.2E-2</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1">
         <f>E2*E4/E7</f>
-        <v>4615384615384.6162</v>
+        <v>1923076923076923</v>
       </c>
       <c r="F8" s="1">
         <f>E8/1000000000000000000</f>
-        <v>4.6153846153846162E-6</v>
+        <v>1.923076923076923E-3</v>
       </c>
       <c r="O8" s="1">
         <f>C2/F8</f>
-        <v>2599999.9999999995</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -792,15 +796,15 @@
       </c>
       <c r="E9" s="1">
         <f>1000000000000000000*2*E2/E6-E8</f>
-        <v>1384615384615.3838</v>
+        <v>576923076923076.5</v>
       </c>
       <c r="F9" s="1">
         <f>E9/1000000000000000000</f>
-        <v>1.3846153846153838E-6</v>
+        <v>5.7692307692307654E-4</v>
       </c>
       <c r="I9" s="1">
         <f>1000000000000000000*(F8-F9)/F6</f>
-        <v>807692.30769230798</v>
+        <v>67307692307.692314</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -815,19 +819,19 @@
       </c>
       <c r="E10" s="1">
         <f>1000000000000000000*(E8-E9)/E6</f>
-        <v>807692.3076923081</v>
+        <v>67307692307.692307</v>
       </c>
       <c r="F10" s="1">
         <f>E10/1000000000000000000</f>
-        <v>8.0769230769230813E-13</v>
+        <v>6.7307692307692306E-8</v>
       </c>
       <c r="H10" s="1">
         <f>(F9-F8)/F6</f>
-        <v>-8.0769230769230803E-13</v>
+        <v>-6.7307692307692319E-8</v>
       </c>
       <c r="K10" s="1">
         <f>H10*1000000000000000000</f>
-        <v>-807692.30769230798</v>
+        <v>-67307692307.692322</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -876,15 +880,15 @@
       </c>
       <c r="E18" s="1">
         <f>E9</f>
-        <v>1384615384615.3838</v>
+        <v>576923076923076.5</v>
       </c>
       <c r="F18" s="1">
         <f>E10*(E17+1000000000000000000)/1000000000000000000</f>
-        <v>3230769230769.2324</v>
+        <v>2.6923076923076922E+17</v>
       </c>
       <c r="G18" s="1">
         <f>E18+F18</f>
-        <v>4615384615384.6162</v>
+        <v>2.6980769230769229E+17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -896,15 +900,15 @@
       </c>
       <c r="E19" s="1">
         <f>E9</f>
-        <v>1384615384615.3838</v>
+        <v>576923076923076.5</v>
       </c>
       <c r="F19" s="1">
         <f>E10*(E17+E16)/1000000000000000000</f>
-        <v>3230769230769.2324</v>
+        <v>2.6923076923076922E+17</v>
       </c>
       <c r="G19" s="1">
         <f>E19+F19</f>
-        <v>4615384615384.6162</v>
+        <v>2.6980769230769229E+17</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -916,7 +920,7 @@
       </c>
       <c r="G20" s="1">
         <f>(G18+G19)/2</f>
-        <v>4615384615384.6162</v>
+        <v>2.6980769230769229E+17</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -928,15 +932,15 @@
       </c>
       <c r="G21" s="1">
         <f>G20*C16</f>
-        <v>4615384615384.6162</v>
+        <v>2.6980769230769229E+17</v>
       </c>
       <c r="H21" s="1">
         <f>G21/1000000000000000000</f>
-        <v>4.6153846153846162E-6</v>
+        <v>0.2698076923076923</v>
       </c>
       <c r="I21" s="6">
         <f>H21*2600/4000000</f>
-        <v>3.0000000000000004E-9</v>
+        <v>1.7537499999999999E-4</v>
       </c>
       <c r="N21">
         <f>(5/2600)*1000000000000000000</f>
@@ -958,10 +962,13 @@
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <f>(F9+F10*C16)</f>
-        <v>1.3846161923076914E-6</v>
+        <v>5.7699038461538424E-4</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>42</v>
+      </c>
       <c r="J29">
         <f>5000000000000000/2600</f>
         <v>1923076923076.9231</v>
@@ -970,7 +977,7 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E33" s="1">
         <f>E9+(E6*E10)/1000000000000000000</f>
-        <v>4615384615384.6162</v>
+        <v>1923076923076923</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
display formats + final price  / base price = 1249
</commit_message>
<xml_diff>
--- a/bonding curve logic.xlsx
+++ b/bonding curve logic.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Praca\web3\turbo-launchpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECD1B1-185E-427B-A718-4E3A3C8D49D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C17C7-205B-43B5-9B6F-359089B08872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B37AC876-497F-4A49-9875-044F50F94948}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{B37AC876-497F-4A49-9875-044F50F94948}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t>Raise target</t>
   </si>
@@ -165,6 +166,63 @@
   </si>
   <si>
     <t>floorprice=1000000000</t>
+  </si>
+  <si>
+    <t>raise Target</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxsupply </t>
+  </si>
+  <si>
+    <t>treshold</t>
+  </si>
+  <si>
+    <t>graduate supply</t>
+  </si>
+  <si>
+    <t>coefficient p/b</t>
+  </si>
+  <si>
+    <t>base price</t>
+  </si>
+  <si>
+    <t>b=2T/(S*(1+c))</t>
+  </si>
+  <si>
+    <t>floor price</t>
+  </si>
+  <si>
+    <t>f=c*b</t>
+  </si>
+  <si>
+    <t>0.0000000009 ETH</t>
+  </si>
+  <si>
+    <t>0.0000000011 ETH</t>
+  </si>
+  <si>
+    <t>maxPrice</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>=(f-b)/S</t>
+  </si>
+  <si>
+    <t>m=b+s*ST</t>
+  </si>
+  <si>
+    <t>fdv</t>
+  </si>
+  <si>
+    <t>=ST*(b+m)/2</t>
   </si>
 </sst>
 </file>
@@ -177,7 +235,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -193,6 +251,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="3">
@@ -237,7 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -247,6 +312,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -584,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5FE277-CB0B-4192-8442-AE2AE9BB3210}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,4 +1062,169 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0624B3BD-A20D-45E8-A783-1188C836EFAD}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="9">
+        <f>C3*C2</f>
+        <v>800000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <f>2*C1/(C4*(1+C5))</f>
+        <v>2.4000000000000001E-11</v>
+      </c>
+      <c r="D7">
+        <f>C7*1000000000000000000</f>
+        <v>24000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <f>C7*C5</f>
+        <v>2.9976000000000003E-8</v>
+      </c>
+      <c r="D8">
+        <f>C8*1000000000000000000</f>
+        <v>29976000000.000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <f>(C8-C7)/C4</f>
+        <v>3.7440000000000004E-17</v>
+      </c>
+      <c r="D13">
+        <f>C13*1000000000000000000</f>
+        <v>37.440000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15">
+        <f>C7+C13*C2</f>
+        <v>3.7464000000000004E-8</v>
+      </c>
+      <c r="D15">
+        <f>D7+D13*C2</f>
+        <v>37464000000.000008</v>
+      </c>
+      <c r="E15">
+        <f>D15/D7</f>
+        <v>1561.0000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <f>C2*(C7+C15)/2</f>
+        <v>18.744000000000003</v>
+      </c>
+      <c r="D17">
+        <f>C2*(D7+D15)/2000000000000000000</f>
+        <v>18.744000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B32" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>